<commit_message>
re-visiting for initial tracer movements
</commit_message>
<xml_diff>
--- a/Surveys/2023/06_17_2023_Tracer_Survey.xlsx
+++ b/Surveys/2023/06_17_2023_Tracer_Survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\RFID_tracers\surveys\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\RFID_tracers\Surveys\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B047534-AD8A-4722-9997-453483D4263F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCECDCD-0F6C-48E9-B42B-19C9EE669F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{69298AC6-6E72-4BA9-9E2C-E826529E513B}"/>
+    <workbookView xWindow="-25320" yWindow="360" windowWidth="25440" windowHeight="15270" xr2:uid="{69298AC6-6E72-4BA9-9E2C-E826529E513B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
   <si>
     <t>Distance from reference point</t>
   </si>
@@ -106,6 +106,9 @@
   <si>
     <t xml:space="preserve">NEW ROCKS </t>
   </si>
+  <si>
+    <t>added on 07-11-2023</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +238,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -400,16 +409,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -424,24 +427,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,13 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -472,7 +451,38 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -498,9 +508,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -538,7 +548,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -644,7 +654,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -786,7 +796,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -796,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0694FFA4-917A-4B6E-97D0-115474C635A2}">
   <dimension ref="A1:P213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H199" sqref="H199"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K207" sqref="K207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,31 +826,31 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="37"/>
+      <c r="H1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -856,37 +866,37 @@
         <v>10</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -906,8 +916,8 @@
       <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
@@ -934,8 +944,8 @@
       <c r="E4" s="7">
         <v>4</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -962,8 +972,8 @@
       <c r="E5" s="4">
         <v>105</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -990,8 +1000,8 @@
       <c r="E6" s="4">
         <v>25</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -1018,8 +1028,8 @@
       <c r="E7" s="4">
         <v>30</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -1046,8 +1056,8 @@
       <c r="E8" s="4">
         <v>88</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -1074,8 +1084,8 @@
       <c r="E9" s="6">
         <v>67</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -1102,8 +1112,8 @@
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -1130,8 +1140,8 @@
       <c r="E11" s="3">
         <v>7</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1152,8 +1162,8 @@
       <c r="E12" s="7">
         <v>113</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -1174,8 +1184,8 @@
       <c r="E13" s="7">
         <v>42</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -1202,8 +1212,8 @@
       <c r="E14" s="7">
         <v>44</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -1224,8 +1234,8 @@
       <c r="E15" s="7">
         <v>5</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1252,8 +1262,8 @@
       <c r="E16" s="4">
         <v>24</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -1274,8 +1284,8 @@
       <c r="E17" s="4">
         <v>99</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -1302,8 +1312,8 @@
       <c r="E18" s="4">
         <v>13</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="5"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1330,8 +1340,8 @@
       <c r="E19" s="4">
         <v>16</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -1358,8 +1368,8 @@
       <c r="E20" s="4">
         <v>112</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1380,8 +1390,8 @@
       <c r="E21" s="8">
         <v>54</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -1402,8 +1412,8 @@
       <c r="E22" s="8">
         <v>38</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -1424,8 +1434,8 @@
       <c r="E23" s="8">
         <v>33</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1446,8 +1456,8 @@
       <c r="E24" s="8">
         <v>117</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -1468,8 +1478,8 @@
       <c r="E25" s="8">
         <v>26</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -1496,8 +1506,8 @@
       <c r="E26" s="8">
         <v>55</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -1518,8 +1528,8 @@
       <c r="E27" s="8">
         <v>32</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -1540,8 +1550,8 @@
       <c r="E28" s="8">
         <v>59</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -1568,8 +1578,8 @@
       <c r="E29" s="8">
         <v>57</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -1590,8 +1600,8 @@
       <c r="E30" s="8">
         <v>104</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -1618,8 +1628,8 @@
       <c r="E31" s="6">
         <v>87</v>
       </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -1640,8 +1650,8 @@
       <c r="E32" s="6">
         <v>72</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -1662,8 +1672,8 @@
       <c r="E33" s="6">
         <v>82</v>
       </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -1690,8 +1700,8 @@
       <c r="E34" s="6">
         <v>71</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -1712,8 +1722,8 @@
       <c r="E35" s="6">
         <v>51</v>
       </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -1740,8 +1750,8 @@
       <c r="E36" s="6">
         <v>80</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -1762,8 +1772,8 @@
       <c r="E37" s="6">
         <v>63</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -1775,17 +1785,17 @@
       <c r="P37" s="14"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="32">
+      <c r="A38" s="24">
         <v>1050</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="32">
+      <c r="E38" s="24">
         <v>1050</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -1797,17 +1807,17 @@
       <c r="P38" s="14"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="32">
+      <c r="A39" s="24">
         <v>1026</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="32">
+      <c r="E39" s="24">
         <v>1026</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -1819,17 +1829,17 @@
       <c r="P39" s="14"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="32">
+      <c r="A40" s="24">
         <v>1055</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="32">
+      <c r="E40" s="24">
         <v>1055</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -1841,17 +1851,17 @@
       <c r="P40" s="14"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="32">
+      <c r="A41" s="24">
         <v>1037</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="32">
+      <c r="E41" s="24">
         <v>1037</v>
       </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -1878,8 +1888,8 @@
       <c r="E42" s="6">
         <v>127</v>
       </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -1900,8 +1910,8 @@
       <c r="E43" s="6">
         <v>134</v>
       </c>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -1922,8 +1932,8 @@
       <c r="E44" s="6">
         <v>79</v>
       </c>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -1935,17 +1945,17 @@
       <c r="P44" s="14"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="32">
+      <c r="A45" s="24">
         <v>1017</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="32">
+      <c r="E45" s="24">
         <v>1017</v>
       </c>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -1957,17 +1967,17 @@
       <c r="P45" s="14"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="32">
+      <c r="A46" s="24">
         <v>1036</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="32">
+      <c r="E46" s="24">
         <v>1036</v>
       </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -1979,17 +1989,17 @@
       <c r="P46" s="14"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="32">
+      <c r="A47" s="24">
         <v>1044</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="32">
+      <c r="E47" s="24">
         <v>1044</v>
       </c>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -2001,7 +2011,7 @@
       <c r="P47" s="14"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="32">
+      <c r="A48" s="24">
         <v>1065</v>
       </c>
       <c r="B48" s="5">
@@ -2013,11 +2023,11 @@
       <c r="D48" s="5">
         <v>4.25</v>
       </c>
-      <c r="E48" s="32">
+      <c r="E48" s="24">
         <v>1065</v>
       </c>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
@@ -2029,15 +2039,15 @@
       <c r="P48" s="14"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="14"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
@@ -2064,8 +2074,8 @@
       <c r="E50" s="3">
         <v>6</v>
       </c>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
@@ -2092,8 +2102,8 @@
       <c r="E51" s="4">
         <v>92</v>
       </c>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
@@ -2120,8 +2130,8 @@
       <c r="E52" s="4">
         <v>96</v>
       </c>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
@@ -2148,8 +2158,8 @@
       <c r="E53" s="4">
         <v>12</v>
       </c>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
@@ -2176,8 +2186,8 @@
       <c r="E54" s="8">
         <v>125</v>
       </c>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -2204,8 +2214,8 @@
       <c r="E55" s="8">
         <v>68</v>
       </c>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
@@ -2226,8 +2236,8 @@
       <c r="E56" s="6">
         <v>86</v>
       </c>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
@@ -2248,8 +2258,8 @@
       <c r="E57" s="6">
         <v>126</v>
       </c>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
@@ -2276,8 +2286,8 @@
       <c r="E58" s="6">
         <v>77</v>
       </c>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
@@ -2298,8 +2308,8 @@
       <c r="E59" s="6">
         <v>76</v>
       </c>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
@@ -2326,8 +2336,8 @@
       <c r="E60" s="6">
         <v>69</v>
       </c>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
@@ -2354,8 +2364,8 @@
       <c r="E61" s="6">
         <v>74</v>
       </c>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
@@ -2367,17 +2377,17 @@
       <c r="P61" s="14"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="32">
+      <c r="A62" s="24">
         <v>1028</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="32">
+      <c r="E62" s="24">
         <v>1028</v>
       </c>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
       <c r="H62" s="14"/>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
@@ -2389,30 +2399,33 @@
       <c r="P62" s="14"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="38">
+      <c r="B63" s="42">
         <v>6</v>
       </c>
-      <c r="C63" s="38">
+      <c r="C63" s="42">
         <v>7</v>
       </c>
-      <c r="D63" s="21">
+      <c r="D63" s="38">
         <v>8</v>
+      </c>
+      <c r="E63" s="43" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>36</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="40">
         <v>1.63</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="40">
         <v>2.02</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64" s="40">
         <v>1.93</v>
       </c>
     </row>
@@ -2420,13 +2433,13 @@
       <c r="A65" s="8">
         <v>107</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="40">
         <v>1.78</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="40">
         <v>2.3800000000000003</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="40">
         <v>2.39</v>
       </c>
     </row>
@@ -2434,13 +2447,13 @@
       <c r="A66" s="8">
         <v>132</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="40">
         <v>1.29</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="40">
         <v>1.95</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66" s="40">
         <v>2.1100000000000003</v>
       </c>
     </row>
@@ -2448,13 +2461,13 @@
       <c r="A67" s="6">
         <v>62</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="40">
         <v>2.66</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67" s="40">
         <v>3.1</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D67" s="40">
         <v>3.06</v>
       </c>
     </row>
@@ -2462,83 +2475,83 @@
       <c r="A68" s="6">
         <v>85</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="40">
         <v>3.2800000000000002</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="40">
         <v>2.8600000000000003</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D68" s="40">
         <v>2.9400000000000004</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="32">
+      <c r="A69" s="24">
         <v>1049</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="40">
         <v>3.45</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C69" s="40">
         <v>4.0200000000000005</v>
       </c>
-      <c r="D69" s="5">
+      <c r="D69" s="40">
         <v>3.9800000000000004</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" s="32">
+      <c r="A70" s="24">
         <v>1052</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="40">
         <v>3.12</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C70" s="40">
         <v>3.6700000000000004</v>
       </c>
-      <c r="D70" s="5">
+      <c r="D70" s="40">
         <v>3.6300000000000003</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B71" s="21">
+      <c r="B71" s="38">
         <v>13</v>
       </c>
-      <c r="C71" s="21">
+      <c r="C71" s="38">
         <v>11</v>
       </c>
-      <c r="D71" s="21">
+      <c r="D71" s="38">
         <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="39">
+      <c r="A72" s="29">
         <v>165</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="40">
         <v>1.27</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="40">
         <v>1.28</v>
       </c>
-      <c r="D72" s="5">
+      <c r="D72" s="40">
         <v>1.22</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="39">
+      <c r="A73" s="29">
         <v>166</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="40">
         <v>1.51</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="40">
         <v>0.71</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="40">
         <v>1.4</v>
       </c>
     </row>
@@ -2546,13 +2559,13 @@
       <c r="A74" s="6">
         <v>138</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="40">
         <v>1.5799999999999998</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="40">
         <v>0.83999999999999986</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D74" s="40">
         <v>1.51</v>
       </c>
     </row>
@@ -2560,55 +2573,55 @@
       <c r="A75" s="4">
         <v>10</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="40">
         <v>1.5799999999999998</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="40">
         <v>0.91999999999999993</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="40">
         <v>1.03</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="40">
+      <c r="A76" s="30">
         <v>150</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="40">
         <v>1.22</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="40">
         <v>0.58000000000000007</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="40">
         <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77" s="40">
+      <c r="A77" s="30">
         <v>156</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="40">
         <v>2.35</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="40">
         <v>1.22</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D77" s="40">
         <v>0.81</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A78" s="40">
+      <c r="A78" s="30">
         <v>157</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="40">
         <v>0.99</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="40">
         <v>0.51</v>
       </c>
-      <c r="D78" s="5">
+      <c r="D78" s="40">
         <v>1.64</v>
       </c>
     </row>
@@ -2616,31 +2629,31 @@
       <c r="A79" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B79" s="28" t="s">
+      <c r="B79" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C79" s="30"/>
-      <c r="D79" s="31"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="36"/>
       <c r="E79" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="26" t="s">
+      <c r="F79" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="26"/>
-      <c r="H79" s="26" t="s">
+      <c r="G79" s="37"/>
+      <c r="H79" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="I79" s="26"/>
-      <c r="J79" s="26"/>
-      <c r="K79" s="26"/>
-      <c r="L79" s="26"/>
-      <c r="M79" s="26" t="s">
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
+      <c r="L79" s="37"/>
+      <c r="M79" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="N79" s="26"/>
-      <c r="O79" s="26"/>
-      <c r="P79" s="26"/>
+      <c r="N79" s="37"/>
+      <c r="O79" s="37"/>
+      <c r="P79" s="37"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
@@ -2656,37 +2669,37 @@
         <v>15</v>
       </c>
       <c r="E80" s="14"/>
-      <c r="F80" s="22" t="s">
+      <c r="F80" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G80" s="22" t="s">
+      <c r="G80" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H80" s="23" t="s">
+      <c r="H80" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I80" s="23" t="s">
+      <c r="I80" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J80" s="23" t="s">
+      <c r="J80" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K80" s="23" t="s">
+      <c r="K80" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="L80" s="23" t="s">
+      <c r="L80" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M80" s="23" t="s">
+      <c r="M80" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N80" s="23" t="s">
+      <c r="N80" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="O80" s="23" t="s">
+      <c r="O80" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P80" s="23" t="s">
+      <c r="P80" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2700,8 +2713,8 @@
       <c r="E81" s="7">
         <v>22</v>
       </c>
-      <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
@@ -2722,8 +2735,8 @@
       <c r="E82" s="7">
         <v>114</v>
       </c>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
@@ -2750,8 +2763,8 @@
       <c r="E83" s="4">
         <v>90</v>
       </c>
-      <c r="F83" s="24"/>
-      <c r="G83" s="24"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
@@ -2778,8 +2791,8 @@
       <c r="E84" s="4">
         <v>19</v>
       </c>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
@@ -2806,8 +2819,8 @@
       <c r="E85" s="4">
         <v>106</v>
       </c>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
@@ -2828,8 +2841,8 @@
       <c r="E86" s="8">
         <v>49</v>
       </c>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
@@ -2856,8 +2869,8 @@
       <c r="E87" s="8">
         <v>128</v>
       </c>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
@@ -2884,8 +2897,8 @@
       <c r="E88" s="8">
         <v>47</v>
       </c>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
@@ -2906,8 +2919,8 @@
       <c r="E89" s="8">
         <v>39</v>
       </c>
-      <c r="F89" s="25"/>
-      <c r="G89" s="24"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="22"/>
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
@@ -2928,8 +2941,8 @@
       <c r="E90" s="8">
         <v>120</v>
       </c>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24"/>
+      <c r="F90" s="22"/>
+      <c r="G90" s="22"/>
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
@@ -2956,8 +2969,8 @@
       <c r="E91" s="8">
         <v>60</v>
       </c>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
@@ -2978,8 +2991,8 @@
       <c r="E92" s="6">
         <v>130</v>
       </c>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
@@ -3006,8 +3019,8 @@
       <c r="E93" s="6">
         <v>123</v>
       </c>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
@@ -3034,8 +3047,8 @@
       <c r="E94" s="6">
         <v>124</v>
       </c>
-      <c r="F94" s="24"/>
-      <c r="G94" s="24"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="22"/>
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
@@ -3056,8 +3069,8 @@
       <c r="E95" s="6">
         <v>81</v>
       </c>
-      <c r="F95" s="24"/>
-      <c r="G95" s="24"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
@@ -3069,17 +3082,17 @@
       <c r="P95" s="14"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A96" s="32">
+      <c r="A96" s="24">
         <v>1006</v>
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
-      <c r="E96" s="32">
+      <c r="E96" s="24">
         <v>1006</v>
       </c>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
       <c r="H96" s="14"/>
       <c r="I96" s="14"/>
       <c r="J96" s="14"/>
@@ -3091,17 +3104,17 @@
       <c r="P96" s="14"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A97" s="32">
+      <c r="A97" s="24">
         <v>1011</v>
       </c>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
-      <c r="E97" s="32">
+      <c r="E97" s="24">
         <v>1011</v>
       </c>
-      <c r="F97" s="24"/>
-      <c r="G97" s="24"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
@@ -3113,17 +3126,17 @@
       <c r="P97" s="14"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A98" s="32">
+      <c r="A98" s="24">
         <v>1048</v>
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
-      <c r="E98" s="32">
+      <c r="E98" s="24">
         <v>1048</v>
       </c>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
       <c r="H98" s="14"/>
       <c r="I98" s="14"/>
       <c r="J98" s="14"/>
@@ -3135,17 +3148,17 @@
       <c r="P98" s="14"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A99" s="32">
+      <c r="A99" s="24">
         <v>1062</v>
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
-      <c r="E99" s="32">
+      <c r="E99" s="24">
         <v>1062</v>
       </c>
-      <c r="F99" s="24"/>
-      <c r="G99" s="24"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
       <c r="H99" s="14"/>
       <c r="I99" s="14"/>
       <c r="J99" s="14"/>
@@ -3163,11 +3176,11 @@
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
-      <c r="E100" s="21" t="s">
+      <c r="E100" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
       <c r="H100" s="14"/>
       <c r="I100" s="14"/>
       <c r="J100" s="14"/>
@@ -3194,8 +3207,8 @@
       <c r="E101" s="7">
         <v>11</v>
       </c>
-      <c r="F101" s="24"/>
-      <c r="G101" s="24"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
@@ -3222,8 +3235,8 @@
       <c r="E102" s="4">
         <v>97</v>
       </c>
-      <c r="F102" s="24"/>
-      <c r="G102" s="24"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
@@ -3250,8 +3263,8 @@
       <c r="E103" s="4">
         <v>37</v>
       </c>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
@@ -3278,8 +3291,8 @@
       <c r="E104" s="8">
         <v>108</v>
       </c>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="22"/>
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="14"/>
@@ -3300,8 +3313,8 @@
       <c r="E105" s="8">
         <v>35</v>
       </c>
-      <c r="F105" s="24"/>
-      <c r="G105" s="24"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="14"/>
@@ -3328,8 +3341,8 @@
       <c r="E106" s="8">
         <v>91</v>
       </c>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24"/>
+      <c r="F106" s="22"/>
+      <c r="G106" s="22"/>
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="14"/>
@@ -3356,8 +3369,8 @@
       <c r="E107" s="8">
         <v>121</v>
       </c>
-      <c r="F107" s="24"/>
-      <c r="G107" s="24"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="22"/>
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="14"/>
@@ -3384,8 +3397,8 @@
       <c r="E108" s="8">
         <v>46</v>
       </c>
-      <c r="F108" s="24"/>
-      <c r="G108" s="24"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="22"/>
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
       <c r="J108" s="14"/>
@@ -3397,17 +3410,17 @@
       <c r="P108" s="14"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A109" s="32">
+      <c r="A109" s="24">
         <v>1051</v>
       </c>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
-      <c r="E109" s="32">
+      <c r="E109" s="24">
         <v>1051</v>
       </c>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="22"/>
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
       <c r="J109" s="14"/>
@@ -3419,17 +3432,17 @@
       <c r="P109" s="14"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A110" s="32">
+      <c r="A110" s="24">
         <v>1042</v>
       </c>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
-      <c r="E110" s="32">
+      <c r="E110" s="24">
         <v>1042</v>
       </c>
-      <c r="F110" s="24"/>
-      <c r="G110" s="24"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
       <c r="H110" s="14"/>
       <c r="I110" s="14"/>
       <c r="J110" s="14"/>
@@ -3450,8 +3463,8 @@
       <c r="E111" s="6">
         <v>131</v>
       </c>
-      <c r="F111" s="24"/>
-      <c r="G111" s="24"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="22"/>
       <c r="H111" s="14"/>
       <c r="I111" s="14"/>
       <c r="J111" s="14"/>
@@ -3478,8 +3491,8 @@
       <c r="E112" s="6">
         <v>75</v>
       </c>
-      <c r="F112" s="24"/>
-      <c r="G112" s="24"/>
+      <c r="F112" s="22"/>
+      <c r="G112" s="22"/>
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
       <c r="J112" s="14"/>
@@ -3491,17 +3504,17 @@
       <c r="P112" s="14"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A113" s="32">
+      <c r="A113" s="24">
         <v>1047</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
-      <c r="E113" s="32">
+      <c r="E113" s="24">
         <v>1047</v>
       </c>
-      <c r="F113" s="24"/>
-      <c r="G113" s="24"/>
+      <c r="F113" s="22"/>
+      <c r="G113" s="22"/>
       <c r="H113" s="14"/>
       <c r="I113" s="14"/>
       <c r="J113" s="14"/>
@@ -3528,8 +3541,8 @@
       <c r="E114" s="6">
         <v>40</v>
       </c>
-      <c r="F114" s="24"/>
-      <c r="G114" s="24"/>
+      <c r="F114" s="22"/>
+      <c r="G114" s="22"/>
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="14"/>
@@ -3550,8 +3563,8 @@
       <c r="E115" s="6">
         <v>118</v>
       </c>
-      <c r="F115" s="24"/>
-      <c r="G115" s="24"/>
+      <c r="F115" s="22"/>
+      <c r="G115" s="22"/>
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="14"/>
@@ -3566,13 +3579,13 @@
       <c r="A116" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B116" s="21">
+      <c r="B116" s="38">
         <v>17</v>
       </c>
-      <c r="C116" s="21">
+      <c r="C116" s="38">
         <v>16</v>
       </c>
-      <c r="D116" s="21">
+      <c r="D116" s="38">
         <v>15</v>
       </c>
     </row>
@@ -3580,13 +3593,13 @@
       <c r="A117" s="4">
         <v>23</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B117" s="40">
         <v>1.3</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C117" s="40">
         <v>2.04</v>
       </c>
-      <c r="D117" s="5">
+      <c r="D117" s="40">
         <v>4.2700000000000005</v>
       </c>
     </row>
@@ -3594,13 +3607,13 @@
       <c r="A118" s="8">
         <v>110</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B118" s="40">
         <v>1.41</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C118" s="40">
         <v>0.74</v>
       </c>
-      <c r="D118" s="5">
+      <c r="D118" s="40">
         <v>3.24</v>
       </c>
     </row>
@@ -3608,13 +3621,13 @@
       <c r="A119" s="8">
         <v>48</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B119" s="40">
         <v>0.82000000000000006</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C119" s="40">
         <v>1.3499999999999999</v>
       </c>
-      <c r="D119" s="5">
+      <c r="D119" s="40">
         <v>2.75</v>
       </c>
     </row>
@@ -3622,13 +3635,13 @@
       <c r="A120" s="6">
         <v>61</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B120" s="40">
         <v>1.6099999999999999</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C120" s="40">
         <v>1.7299999999999998</v>
       </c>
-      <c r="D120" s="5">
+      <c r="D120" s="40">
         <v>1.72</v>
       </c>
     </row>
@@ -3636,55 +3649,55 @@
       <c r="A121" s="6">
         <v>52</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B121" s="40">
         <v>1.41</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C121" s="40">
         <v>1.25</v>
       </c>
-      <c r="D121" s="5">
+      <c r="D121" s="40">
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A122" s="32">
+      <c r="A122" s="24">
         <v>1061</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B122" s="40">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C122" s="40">
         <v>2.1500000000000004</v>
       </c>
-      <c r="D122" s="5">
+      <c r="D122" s="40">
         <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="123" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="32">
+      <c r="A123" s="24">
         <v>1040</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B123" s="40">
         <v>2.77</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C123" s="40">
         <v>1.7</v>
       </c>
-      <c r="D123" s="5">
+      <c r="D123" s="40">
         <v>1.91</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A124" s="32">
+      <c r="A124" s="24">
         <v>1053</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B124" s="40">
         <v>1.74</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C124" s="40">
         <v>1.01</v>
       </c>
-      <c r="D124" s="5">
+      <c r="D124" s="40">
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -3692,27 +3705,30 @@
       <c r="A125" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B125" s="21">
+      <c r="B125" s="38">
         <v>17</v>
       </c>
-      <c r="C125" s="21">
+      <c r="C125" s="38">
         <v>16</v>
       </c>
-      <c r="D125" s="21">
+      <c r="D125" s="38">
         <v>15</v>
+      </c>
+      <c r="E125" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="6">
         <v>139</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B126" s="40">
         <v>0.75</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C126" s="40">
         <v>1.3399999999999999</v>
       </c>
-      <c r="D126" s="5">
+      <c r="D126" s="40">
         <v>3.2</v>
       </c>
     </row>
@@ -3720,13 +3736,13 @@
       <c r="A127" s="6">
         <v>142</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B127" s="40">
         <v>1.38</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C127" s="40">
         <v>0.72</v>
       </c>
-      <c r="D127" s="5">
+      <c r="D127" s="40">
         <v>2.85</v>
       </c>
     </row>
@@ -3734,13 +3750,13 @@
       <c r="A128" s="6">
         <v>146</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128" s="40">
         <v>1.32</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C128" s="40">
         <v>1.0799999999999998</v>
       </c>
-      <c r="D128" s="5">
+      <c r="D128" s="40">
         <v>3.5900000000000003</v>
       </c>
     </row>
@@ -3748,13 +3764,13 @@
       <c r="A129" s="6">
         <v>149</v>
       </c>
-      <c r="B129" s="5">
+      <c r="B129" s="40">
         <v>1.05</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C129" s="40">
         <v>0.98</v>
       </c>
-      <c r="D129" s="5">
+      <c r="D129" s="40">
         <v>3.0900000000000003</v>
       </c>
     </row>
@@ -3762,13 +3778,13 @@
       <c r="A130" s="8">
         <v>158</v>
       </c>
-      <c r="B130" s="5">
+      <c r="B130" s="40">
         <v>1.05</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C130" s="40">
         <v>1.01</v>
       </c>
-      <c r="D130" s="5">
+      <c r="D130" s="40">
         <v>2.89</v>
       </c>
     </row>
@@ -3776,27 +3792,27 @@
       <c r="A131" s="8">
         <v>164</v>
       </c>
-      <c r="B131" s="5">
+      <c r="B131" s="40">
         <v>1.28</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C131" s="40">
         <v>1.18</v>
       </c>
-      <c r="D131" s="5">
+      <c r="D131" s="40">
         <v>3.7</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A132" s="41">
+      <c r="A132" s="31">
         <v>154</v>
       </c>
-      <c r="B132" s="5">
+      <c r="B132" s="40">
         <v>0.8899999999999999</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C132" s="40">
         <v>1.38</v>
       </c>
-      <c r="D132" s="5">
+      <c r="D132" s="40">
         <v>3.5100000000000002</v>
       </c>
     </row>
@@ -3804,13 +3820,13 @@
       <c r="A133" s="3">
         <v>169</v>
       </c>
-      <c r="B133" s="5">
+      <c r="B133" s="40">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C133" s="40">
         <v>1.45</v>
       </c>
-      <c r="D133" s="5">
+      <c r="D133" s="40">
         <v>3.8500000000000005</v>
       </c>
     </row>
@@ -3818,34 +3834,34 @@
       <c r="A134" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C134" s="19"/>
-      <c r="D134" s="20"/>
-      <c r="E134" s="21" t="s">
+      <c r="C134" s="18"/>
+      <c r="D134" s="19"/>
+      <c r="E134" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F134" s="23" t="s">
+      <c r="F134" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G134" s="23"/>
-      <c r="H134" s="23" t="s">
+      <c r="G134" s="21"/>
+      <c r="H134" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I134" s="23"/>
-      <c r="J134" s="23"/>
-      <c r="K134" s="23"/>
-      <c r="L134" s="23"/>
-      <c r="M134" s="23" t="s">
+      <c r="I134" s="21"/>
+      <c r="J134" s="21"/>
+      <c r="K134" s="21"/>
+      <c r="L134" s="21"/>
+      <c r="M134" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N134" s="23"/>
-      <c r="O134" s="23"/>
-      <c r="P134" s="23"/>
+      <c r="N134" s="21"/>
+      <c r="O134" s="21"/>
+      <c r="P134" s="21"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A135" s="21" t="s">
+      <c r="A135" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B135" s="5">
@@ -3858,37 +3874,37 @@
         <v>21</v>
       </c>
       <c r="E135" s="5"/>
-      <c r="F135" s="22" t="s">
+      <c r="F135" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G135" s="22" t="s">
+      <c r="G135" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H135" s="23" t="s">
+      <c r="H135" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I135" s="23" t="s">
+      <c r="I135" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J135" s="23" t="s">
+      <c r="J135" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K135" s="23" t="s">
+      <c r="K135" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="L135" s="23" t="s">
+      <c r="L135" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M135" s="23" t="s">
+      <c r="M135" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N135" s="23" t="s">
+      <c r="N135" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="O135" s="23" t="s">
+      <c r="O135" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P135" s="23" t="s">
+      <c r="P135" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3902,8 +3918,8 @@
       <c r="E136" s="3">
         <v>8</v>
       </c>
-      <c r="F136" s="24"/>
-      <c r="G136" s="24"/>
+      <c r="F136" s="22"/>
+      <c r="G136" s="22"/>
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
       <c r="J136" s="14"/>
@@ -3924,8 +3940,8 @@
       <c r="E137" s="7">
         <v>2</v>
       </c>
-      <c r="F137" s="24"/>
-      <c r="G137" s="24"/>
+      <c r="F137" s="22"/>
+      <c r="G137" s="22"/>
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
       <c r="J137" s="14"/>
@@ -3946,8 +3962,8 @@
       <c r="E138" s="7">
         <v>43</v>
       </c>
-      <c r="F138" s="24"/>
-      <c r="G138" s="24"/>
+      <c r="F138" s="22"/>
+      <c r="G138" s="22"/>
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
       <c r="J138" s="14"/>
@@ -3974,8 +3990,8 @@
       <c r="E139" s="4">
         <v>15</v>
       </c>
-      <c r="F139" s="24"/>
-      <c r="G139" s="24"/>
+      <c r="F139" s="22"/>
+      <c r="G139" s="22"/>
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
       <c r="J139" s="14"/>
@@ -3996,8 +4012,8 @@
       <c r="E140" s="4">
         <v>94</v>
       </c>
-      <c r="F140" s="24"/>
-      <c r="G140" s="24"/>
+      <c r="F140" s="22"/>
+      <c r="G140" s="22"/>
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
       <c r="J140" s="14"/>
@@ -4018,8 +4034,8 @@
       <c r="E141" s="4">
         <v>95</v>
       </c>
-      <c r="F141" s="24"/>
-      <c r="G141" s="24"/>
+      <c r="F141" s="22"/>
+      <c r="G141" s="22"/>
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
       <c r="J141" s="14"/>
@@ -4040,8 +4056,8 @@
       <c r="E142" s="8">
         <v>109</v>
       </c>
-      <c r="F142" s="24"/>
-      <c r="G142" s="24"/>
+      <c r="F142" s="22"/>
+      <c r="G142" s="22"/>
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
       <c r="J142" s="14"/>
@@ -4062,8 +4078,8 @@
       <c r="E143" s="8">
         <v>66</v>
       </c>
-      <c r="F143" s="24"/>
-      <c r="G143" s="24"/>
+      <c r="F143" s="22"/>
+      <c r="G143" s="22"/>
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
       <c r="J143" s="14"/>
@@ -4084,8 +4100,8 @@
       <c r="E144" s="6">
         <v>73</v>
       </c>
-      <c r="F144" s="24"/>
-      <c r="G144" s="24"/>
+      <c r="F144" s="22"/>
+      <c r="G144" s="22"/>
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
       <c r="J144" s="14"/>
@@ -4106,8 +4122,8 @@
       <c r="E145" s="6">
         <v>129</v>
       </c>
-      <c r="F145" s="24"/>
-      <c r="G145" s="24"/>
+      <c r="F145" s="22"/>
+      <c r="G145" s="22"/>
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
       <c r="J145" s="14"/>
@@ -4128,8 +4144,8 @@
       <c r="E146" s="6">
         <v>70</v>
       </c>
-      <c r="F146" s="24"/>
-      <c r="G146" s="24"/>
+      <c r="F146" s="22"/>
+      <c r="G146" s="22"/>
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
       <c r="J146" s="14"/>
@@ -4150,8 +4166,8 @@
       <c r="E147" s="6">
         <v>58</v>
       </c>
-      <c r="F147" s="24"/>
-      <c r="G147" s="24"/>
+      <c r="F147" s="22"/>
+      <c r="G147" s="22"/>
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
       <c r="J147" s="14"/>
@@ -4178,8 +4194,8 @@
       <c r="E148" s="6">
         <v>136</v>
       </c>
-      <c r="F148" s="24"/>
-      <c r="G148" s="24"/>
+      <c r="F148" s="22"/>
+      <c r="G148" s="22"/>
       <c r="H148" s="14"/>
       <c r="I148" s="14"/>
       <c r="J148" s="14"/>
@@ -4191,7 +4207,7 @@
       <c r="P148" s="14"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A149" s="32">
+      <c r="A149" s="24">
         <v>1039</v>
       </c>
       <c r="B149" s="5">
@@ -4203,11 +4219,11 @@
       <c r="D149" s="5">
         <v>2.9200000000000004</v>
       </c>
-      <c r="E149" s="32">
+      <c r="E149" s="24">
         <v>1039</v>
       </c>
-      <c r="F149" s="24"/>
-      <c r="G149" s="24"/>
+      <c r="F149" s="22"/>
+      <c r="G149" s="22"/>
       <c r="H149" s="14"/>
       <c r="I149" s="14"/>
       <c r="J149" s="14"/>
@@ -4219,17 +4235,17 @@
       <c r="P149" s="14"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A150" s="32">
+      <c r="A150" s="24">
         <v>1005</v>
       </c>
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
-      <c r="E150" s="32">
+      <c r="E150" s="24">
         <v>1005</v>
       </c>
-      <c r="F150" s="24"/>
-      <c r="G150" s="24"/>
+      <c r="F150" s="22"/>
+      <c r="G150" s="22"/>
       <c r="H150" s="14"/>
       <c r="I150" s="14"/>
       <c r="J150" s="14"/>
@@ -4241,17 +4257,17 @@
       <c r="P150" s="14"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A151" s="32">
+      <c r="A151" s="24">
         <v>1031</v>
       </c>
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
-      <c r="E151" s="32">
+      <c r="E151" s="24">
         <v>1031</v>
       </c>
-      <c r="F151" s="24"/>
-      <c r="G151" s="24"/>
+      <c r="F151" s="22"/>
+      <c r="G151" s="22"/>
       <c r="H151" s="14"/>
       <c r="I151" s="14"/>
       <c r="J151" s="14"/>
@@ -4263,17 +4279,17 @@
       <c r="P151" s="14"/>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A152" s="32">
+      <c r="A152" s="24">
         <v>1010</v>
       </c>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
-      <c r="E152" s="32">
+      <c r="E152" s="24">
         <v>1010</v>
       </c>
-      <c r="F152" s="24"/>
-      <c r="G152" s="24"/>
+      <c r="F152" s="22"/>
+      <c r="G152" s="22"/>
       <c r="H152" s="14"/>
       <c r="I152" s="14"/>
       <c r="J152" s="14"/>
@@ -4285,278 +4301,281 @@
       <c r="P152" s="14"/>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B153" s="36">
+      <c r="B153" s="41">
         <v>21</v>
       </c>
-      <c r="C153" s="36">
+      <c r="C153" s="41">
         <v>20</v>
       </c>
-      <c r="D153" s="36">
+      <c r="D153" s="41">
         <v>19</v>
+      </c>
+      <c r="E153" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>140</v>
       </c>
-      <c r="B154" s="5">
+      <c r="B154" s="40">
         <v>1.86</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C154" s="40">
         <v>1.47</v>
       </c>
-      <c r="D154" s="5">
+      <c r="D154" s="40">
         <v>1.25</v>
       </c>
-      <c r="F154" s="35"/>
-      <c r="G154" s="35"/>
-      <c r="H154" s="35"/>
+      <c r="F154" s="27"/>
+      <c r="G154" s="27"/>
+      <c r="H154" s="27"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="6">
         <v>143</v>
       </c>
-      <c r="B155" s="5">
+      <c r="B155" s="40">
         <v>1.84</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C155" s="40">
         <v>1.56</v>
       </c>
-      <c r="D155" s="5">
+      <c r="D155" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="F155" s="35"/>
-      <c r="G155" s="35"/>
-      <c r="H155" s="35"/>
+      <c r="F155" s="27"/>
+      <c r="G155" s="27"/>
+      <c r="H155" s="27"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="6">
         <v>145</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B156" s="40">
         <v>1.41</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C156" s="40">
         <v>0.90999999999999992</v>
       </c>
-      <c r="D156" s="5">
+      <c r="D156" s="40">
         <v>1.43</v>
       </c>
-      <c r="F156" s="35"/>
-      <c r="G156" s="35"/>
-      <c r="H156" s="35"/>
+      <c r="F156" s="27"/>
+      <c r="G156" s="27"/>
+      <c r="H156" s="27"/>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="6">
         <v>147</v>
       </c>
-      <c r="B157" s="5">
+      <c r="B157" s="40">
         <v>1.7499999999999998</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C157" s="40">
         <v>1.18</v>
       </c>
-      <c r="D157" s="5">
+      <c r="D157" s="40">
         <v>2.81</v>
       </c>
-      <c r="F157" s="35"/>
-      <c r="G157" s="35"/>
-      <c r="H157" s="35"/>
+      <c r="F157" s="27"/>
+      <c r="G157" s="27"/>
+      <c r="H157" s="27"/>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="8">
         <v>160</v>
       </c>
-      <c r="B158" s="5">
+      <c r="B158" s="40">
         <v>1.25</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C158" s="40">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D158" s="5">
+      <c r="D158" s="40">
         <v>1.19</v>
       </c>
-      <c r="F158" s="35"/>
-      <c r="G158" s="35"/>
-      <c r="H158" s="35"/>
+      <c r="F158" s="27"/>
+      <c r="G158" s="27"/>
+      <c r="H158" s="27"/>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="8">
         <v>162</v>
       </c>
-      <c r="B159" s="5">
+      <c r="B159" s="40">
         <v>1.0899999999999999</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C159" s="40">
         <v>0.8899999999999999</v>
       </c>
-      <c r="D159" s="5">
+      <c r="D159" s="40">
         <v>1.86</v>
       </c>
-      <c r="F159" s="35"/>
-      <c r="G159" s="35"/>
-      <c r="H159" s="35"/>
+      <c r="F159" s="27"/>
+      <c r="G159" s="27"/>
+      <c r="H159" s="27"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>18</v>
       </c>
-      <c r="B160" s="5">
+      <c r="B160" s="40">
         <v>1.5</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C160" s="40">
         <v>1.05</v>
       </c>
-      <c r="D160" s="5">
+      <c r="D160" s="40">
         <v>2.52</v>
       </c>
-      <c r="F160" s="35"/>
-      <c r="G160" s="35"/>
-      <c r="H160" s="35"/>
+      <c r="F160" s="27"/>
+      <c r="G160" s="27"/>
+      <c r="H160" s="27"/>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>170</v>
       </c>
-      <c r="B161" s="5">
+      <c r="B161" s="40">
         <v>1.45</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C161" s="40">
         <v>0.87999999999999989</v>
       </c>
-      <c r="D161" s="5">
+      <c r="D161" s="40">
         <v>1.48</v>
       </c>
-      <c r="F161" s="35"/>
-      <c r="G161" s="35"/>
-      <c r="H161" s="35"/>
+      <c r="F161" s="27"/>
+      <c r="G161" s="27"/>
+      <c r="H161" s="27"/>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A162" s="41">
+      <c r="A162" s="31">
         <v>155</v>
       </c>
-      <c r="B162" s="5">
+      <c r="B162" s="40">
         <v>1.52</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C162" s="40">
         <v>0.89999999999999991</v>
       </c>
-      <c r="D162" s="5">
+      <c r="D162" s="40">
         <v>1.47</v>
       </c>
-      <c r="F162" s="35"/>
-      <c r="G162" s="35"/>
-      <c r="H162" s="35"/>
+      <c r="F162" s="27"/>
+      <c r="G162" s="27"/>
+      <c r="H162" s="27"/>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A163" s="41">
+      <c r="A163" s="31">
         <v>152</v>
       </c>
-      <c r="B163" s="5">
+      <c r="B163" s="40">
         <v>1.01</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C163" s="40">
         <v>1.19</v>
       </c>
-      <c r="D163" s="5">
+      <c r="D163" s="40">
         <v>2.1</v>
       </c>
-      <c r="F163" s="35"/>
-      <c r="G163" s="35"/>
-      <c r="H163" s="35"/>
+      <c r="F163" s="27"/>
+      <c r="G163" s="27"/>
+      <c r="H163" s="27"/>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>168</v>
       </c>
-      <c r="B164" s="5">
+      <c r="B164" s="40">
         <v>1.53</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C164" s="40">
         <v>1.53</v>
       </c>
-      <c r="D164" s="5">
+      <c r="D164" s="40">
         <v>2.8000000000000003</v>
       </c>
-      <c r="F164" s="35"/>
-      <c r="G164" s="35"/>
-      <c r="H164" s="35"/>
+      <c r="F164" s="27"/>
+      <c r="G164" s="27"/>
+      <c r="H164" s="27"/>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B165" s="18" t="s">
+      <c r="B165" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C165" s="19"/>
-      <c r="D165" s="20"/>
-      <c r="E165" s="21" t="s">
+      <c r="C165" s="18"/>
+      <c r="D165" s="19"/>
+      <c r="E165" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F165" s="23" t="s">
+      <c r="F165" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G165" s="23"/>
-      <c r="H165" s="23" t="s">
+      <c r="G165" s="21"/>
+      <c r="H165" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I165" s="23"/>
-      <c r="J165" s="23"/>
-      <c r="K165" s="23"/>
-      <c r="L165" s="23"/>
-      <c r="M165" s="23" t="s">
+      <c r="I165" s="21"/>
+      <c r="J165" s="21"/>
+      <c r="K165" s="21"/>
+      <c r="L165" s="21"/>
+      <c r="M165" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N165" s="23"/>
-      <c r="O165" s="23"/>
-      <c r="P165" s="23"/>
+      <c r="N165" s="21"/>
+      <c r="O165" s="21"/>
+      <c r="P165" s="21"/>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A166" s="21" t="s">
+      <c r="A166" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B166" s="21">
+      <c r="B166" s="2">
         <v>29</v>
       </c>
-      <c r="C166" s="21">
+      <c r="C166" s="2">
         <v>27</v>
       </c>
-      <c r="D166" s="21">
+      <c r="D166" s="2">
         <v>28</v>
       </c>
-      <c r="E166" s="33"/>
-      <c r="F166" s="22" t="s">
+      <c r="E166" s="25"/>
+      <c r="F166" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G166" s="22" t="s">
+      <c r="G166" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H166" s="23" t="s">
+      <c r="H166" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I166" s="23" t="s">
+      <c r="I166" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J166" s="23" t="s">
+      <c r="J166" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K166" s="23" t="s">
+      <c r="K166" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="L166" s="23" t="s">
+      <c r="L166" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M166" s="23" t="s">
+      <c r="M166" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N166" s="23" t="s">
+      <c r="N166" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="O166" s="23" t="s">
+      <c r="O166" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P166" s="23" t="s">
+      <c r="P166" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4576,8 +4595,8 @@
       <c r="E167" s="3">
         <v>1</v>
       </c>
-      <c r="F167" s="24"/>
-      <c r="G167" s="24"/>
+      <c r="F167" s="22"/>
+      <c r="G167" s="22"/>
       <c r="H167" s="14"/>
       <c r="I167" s="14"/>
       <c r="J167" s="14"/>
@@ -4598,8 +4617,8 @@
       <c r="E168" s="7">
         <v>41</v>
       </c>
-      <c r="F168" s="24"/>
-      <c r="G168" s="24"/>
+      <c r="F168" s="22"/>
+      <c r="G168" s="22"/>
       <c r="H168" s="14"/>
       <c r="I168" s="14"/>
       <c r="J168" s="14"/>
@@ -4626,8 +4645,8 @@
       <c r="E169" s="4">
         <v>17</v>
       </c>
-      <c r="F169" s="24"/>
-      <c r="G169" s="24"/>
+      <c r="F169" s="22"/>
+      <c r="G169" s="22"/>
       <c r="H169" s="14"/>
       <c r="I169" s="14"/>
       <c r="J169" s="14"/>
@@ -4648,8 +4667,8 @@
       <c r="E170" s="4">
         <v>29</v>
       </c>
-      <c r="F170" s="24"/>
-      <c r="G170" s="24"/>
+      <c r="F170" s="22"/>
+      <c r="G170" s="22"/>
       <c r="H170" s="14"/>
       <c r="I170" s="14"/>
       <c r="J170" s="14"/>
@@ -4670,8 +4689,8 @@
       <c r="E171" s="4">
         <v>14</v>
       </c>
-      <c r="F171" s="24"/>
-      <c r="G171" s="24"/>
+      <c r="F171" s="22"/>
+      <c r="G171" s="22"/>
       <c r="H171" s="14"/>
       <c r="I171" s="14"/>
       <c r="J171" s="14"/>
@@ -4698,8 +4717,8 @@
       <c r="E172" s="8">
         <v>119</v>
       </c>
-      <c r="F172" s="24"/>
-      <c r="G172" s="24"/>
+      <c r="F172" s="22"/>
+      <c r="G172" s="22"/>
       <c r="H172" s="14"/>
       <c r="I172" s="14"/>
       <c r="J172" s="14"/>
@@ -4720,8 +4739,8 @@
       <c r="E173" s="8">
         <v>45</v>
       </c>
-      <c r="F173" s="24"/>
-      <c r="G173" s="24"/>
+      <c r="F173" s="22"/>
+      <c r="G173" s="22"/>
       <c r="H173" s="14"/>
       <c r="I173" s="14"/>
       <c r="J173" s="14"/>
@@ -4748,8 +4767,8 @@
       <c r="E174" s="8">
         <v>20</v>
       </c>
-      <c r="F174" s="24"/>
-      <c r="G174" s="24"/>
+      <c r="F174" s="22"/>
+      <c r="G174" s="22"/>
       <c r="H174" s="14"/>
       <c r="I174" s="14"/>
       <c r="J174" s="14"/>
@@ -4770,8 +4789,8 @@
       <c r="E175" s="8">
         <v>34</v>
       </c>
-      <c r="F175" s="24"/>
-      <c r="G175" s="24"/>
+      <c r="F175" s="22"/>
+      <c r="G175" s="22"/>
       <c r="H175" s="14"/>
       <c r="I175" s="14"/>
       <c r="J175" s="14"/>
@@ -4792,8 +4811,8 @@
       <c r="E176" s="6">
         <v>64</v>
       </c>
-      <c r="F176" s="24"/>
-      <c r="G176" s="24"/>
+      <c r="F176" s="22"/>
+      <c r="G176" s="22"/>
       <c r="H176" s="14"/>
       <c r="I176" s="14"/>
       <c r="J176" s="14"/>
@@ -4814,8 +4833,8 @@
       <c r="E177" s="6">
         <v>56</v>
       </c>
-      <c r="F177" s="24"/>
-      <c r="G177" s="24"/>
+      <c r="F177" s="22"/>
+      <c r="G177" s="22"/>
       <c r="H177" s="14"/>
       <c r="I177" s="14"/>
       <c r="J177" s="14"/>
@@ -4836,8 +4855,8 @@
       <c r="E178" s="6">
         <v>78</v>
       </c>
-      <c r="F178" s="24"/>
-      <c r="G178" s="24"/>
+      <c r="F178" s="22"/>
+      <c r="G178" s="22"/>
       <c r="H178" s="14"/>
       <c r="I178" s="14"/>
       <c r="J178" s="14"/>
@@ -4849,17 +4868,17 @@
       <c r="P178" s="14"/>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A179" s="32">
+      <c r="A179" s="24">
         <v>1002</v>
       </c>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
-      <c r="E179" s="32">
+      <c r="E179" s="24">
         <v>1002</v>
       </c>
-      <c r="F179" s="24"/>
-      <c r="G179" s="24"/>
+      <c r="F179" s="22"/>
+      <c r="G179" s="22"/>
       <c r="H179" s="14"/>
       <c r="I179" s="14"/>
       <c r="J179" s="14"/>
@@ -4871,17 +4890,17 @@
       <c r="P179" s="14"/>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A180" s="32">
+      <c r="A180" s="24">
         <v>1014</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
-      <c r="E180" s="32">
+      <c r="E180" s="24">
         <v>1014</v>
       </c>
-      <c r="F180" s="24"/>
-      <c r="G180" s="24"/>
+      <c r="F180" s="22"/>
+      <c r="G180" s="22"/>
       <c r="H180" s="14"/>
       <c r="I180" s="14"/>
       <c r="J180" s="14"/>
@@ -4893,17 +4912,17 @@
       <c r="P180" s="14"/>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A181" s="32">
+      <c r="A181" s="24">
         <v>1043</v>
       </c>
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
-      <c r="E181" s="32">
+      <c r="E181" s="24">
         <v>1043</v>
       </c>
-      <c r="F181" s="24"/>
-      <c r="G181" s="24"/>
+      <c r="F181" s="22"/>
+      <c r="G181" s="22"/>
       <c r="H181" s="14"/>
       <c r="I181" s="14"/>
       <c r="J181" s="14"/>
@@ -4915,17 +4934,17 @@
       <c r="P181" s="14"/>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A182" s="32">
+      <c r="A182" s="24">
         <v>1058</v>
       </c>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
-      <c r="E182" s="32">
+      <c r="E182" s="24">
         <v>1058</v>
       </c>
-      <c r="F182" s="24"/>
-      <c r="G182" s="24"/>
+      <c r="F182" s="22"/>
+      <c r="G182" s="22"/>
       <c r="H182" s="14"/>
       <c r="I182" s="14"/>
       <c r="J182" s="14"/>
@@ -4937,15 +4956,15 @@
       <c r="P182" s="14"/>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A183" s="29" t="s">
+      <c r="A183" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B183" s="29"/>
-      <c r="C183" s="29"/>
-      <c r="D183" s="29"/>
-      <c r="E183" s="34"/>
-      <c r="F183" s="24"/>
-      <c r="G183" s="24"/>
+      <c r="B183" s="32"/>
+      <c r="C183" s="32"/>
+      <c r="D183" s="32"/>
+      <c r="E183" s="26"/>
+      <c r="F183" s="22"/>
+      <c r="G183" s="22"/>
       <c r="H183" s="14"/>
       <c r="I183" s="14"/>
       <c r="J183" s="14"/>
@@ -4972,8 +4991,8 @@
       <c r="E184" s="7">
         <v>9</v>
       </c>
-      <c r="F184" s="24"/>
-      <c r="G184" s="24"/>
+      <c r="F184" s="22"/>
+      <c r="G184" s="22"/>
       <c r="H184" s="14"/>
       <c r="I184" s="14"/>
       <c r="J184" s="14"/>
@@ -5000,8 +5019,8 @@
       <c r="E185" s="4">
         <v>111</v>
       </c>
-      <c r="F185" s="24"/>
-      <c r="G185" s="24"/>
+      <c r="F185" s="22"/>
+      <c r="G185" s="22"/>
       <c r="H185" s="14"/>
       <c r="I185" s="14"/>
       <c r="J185" s="14"/>
@@ -5028,8 +5047,8 @@
       <c r="E186" s="8">
         <v>89</v>
       </c>
-      <c r="F186" s="24"/>
-      <c r="G186" s="24"/>
+      <c r="F186" s="22"/>
+      <c r="G186" s="22"/>
       <c r="H186" s="14"/>
       <c r="I186" s="14"/>
       <c r="J186" s="14"/>
@@ -5050,8 +5069,8 @@
       <c r="E187" s="8">
         <v>68</v>
       </c>
-      <c r="F187" s="24"/>
-      <c r="G187" s="24"/>
+      <c r="F187" s="22"/>
+      <c r="G187" s="22"/>
       <c r="H187" s="14"/>
       <c r="I187" s="14"/>
       <c r="J187" s="14"/>
@@ -5078,8 +5097,8 @@
       <c r="E188" s="8">
         <v>102</v>
       </c>
-      <c r="F188" s="24"/>
-      <c r="G188" s="24"/>
+      <c r="F188" s="22"/>
+      <c r="G188" s="22"/>
       <c r="H188" s="14"/>
       <c r="I188" s="14"/>
       <c r="J188" s="14"/>
@@ -5106,8 +5125,8 @@
       <c r="E189" s="8">
         <v>116</v>
       </c>
-      <c r="F189" s="24"/>
-      <c r="G189" s="24"/>
+      <c r="F189" s="22"/>
+      <c r="G189" s="22"/>
       <c r="H189" s="14"/>
       <c r="I189" s="14"/>
       <c r="J189" s="14"/>
@@ -5134,8 +5153,8 @@
       <c r="E190" s="9">
         <v>122</v>
       </c>
-      <c r="F190" s="24"/>
-      <c r="G190" s="24"/>
+      <c r="F190" s="22"/>
+      <c r="G190" s="22"/>
       <c r="H190" s="14"/>
       <c r="I190" s="14"/>
       <c r="J190" s="14"/>
@@ -5162,8 +5181,8 @@
       <c r="E191" s="9">
         <v>135</v>
       </c>
-      <c r="F191" s="24"/>
-      <c r="G191" s="24"/>
+      <c r="F191" s="22"/>
+      <c r="G191" s="22"/>
       <c r="H191" s="14"/>
       <c r="I191" s="14"/>
       <c r="J191" s="14"/>
@@ -5175,308 +5194,314 @@
       <c r="P191" s="14"/>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B192" s="42">
+      <c r="B192" s="38">
         <v>29</v>
       </c>
-      <c r="C192" s="42">
+      <c r="C192" s="38">
         <v>28</v>
       </c>
-      <c r="D192" s="42">
+      <c r="D192" s="38">
         <v>27</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="6">
         <v>137</v>
       </c>
-      <c r="B193" s="5">
+      <c r="B193" s="40">
         <v>2.4000000000000004</v>
       </c>
-      <c r="C193" s="5">
+      <c r="C193" s="40">
         <v>0.5</v>
       </c>
-      <c r="D193" s="5">
+      <c r="D193" s="40">
         <v>2.54</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="6">
         <v>141</v>
       </c>
-      <c r="B194" s="5">
+      <c r="B194" s="40">
         <v>2.16</v>
       </c>
-      <c r="C194" s="5">
+      <c r="C194" s="40">
         <v>0.66999999999999993</v>
       </c>
-      <c r="D194" s="5">
+      <c r="D194" s="40">
         <v>1.7899999999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="6">
         <v>144</v>
       </c>
-      <c r="B195" s="5">
+      <c r="B195" s="40">
         <v>1.78</v>
       </c>
-      <c r="C195" s="5">
+      <c r="C195" s="40">
         <v>0.8</v>
       </c>
-      <c r="D195" s="5">
+      <c r="D195" s="40">
         <v>1.7099999999999997</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="6">
         <v>148</v>
       </c>
-      <c r="B196" s="5">
+      <c r="B196" s="40">
         <v>1.55</v>
       </c>
-      <c r="C196" s="5">
+      <c r="C196" s="40">
         <v>1.0899999999999999</v>
       </c>
-      <c r="D196" s="5">
+      <c r="D196" s="40">
         <v>1.8699999999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="8">
         <v>159</v>
       </c>
-      <c r="B197" s="5">
+      <c r="B197" s="40">
         <v>2.27</v>
       </c>
-      <c r="C197" s="5">
+      <c r="C197" s="40">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D197" s="5">
+      <c r="D197" s="40">
         <v>2.1700000000000004</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="8">
         <v>161</v>
       </c>
-      <c r="B198" s="5">
+      <c r="B198" s="40">
         <v>2.1100000000000003</v>
       </c>
-      <c r="C198" s="5">
+      <c r="C198" s="40">
         <v>0.95</v>
       </c>
-      <c r="D198" s="5">
+      <c r="D198" s="40">
         <v>1.5899999999999999</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="8">
         <v>163</v>
       </c>
-      <c r="B199" s="5">
+      <c r="B199" s="40">
         <v>2.21</v>
       </c>
-      <c r="C199" s="5">
+      <c r="C199" s="40">
         <v>0.65999999999999992</v>
       </c>
-      <c r="D199" s="5">
+      <c r="D199" s="40">
         <v>2.3400000000000003</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>101</v>
       </c>
-      <c r="B200" s="5">
+      <c r="B200" s="40">
         <v>1.66</v>
       </c>
-      <c r="C200" s="5">
+      <c r="C200" s="40">
         <v>0.90999999999999992</v>
       </c>
-      <c r="D200" s="5">
+      <c r="D200" s="40">
         <v>1.82</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="41">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="31">
         <v>151</v>
       </c>
-      <c r="B201" s="5">
+      <c r="B201" s="40">
         <v>2.3000000000000003</v>
       </c>
-      <c r="C201" s="5">
+      <c r="C201" s="40">
         <v>0.26000000000000006</v>
       </c>
-      <c r="D201" s="5">
+      <c r="D201" s="40">
         <v>2.27</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="41">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="31">
         <v>153</v>
       </c>
-      <c r="B202" s="5">
+      <c r="B202" s="40">
         <v>1.54</v>
       </c>
-      <c r="C202" s="5">
+      <c r="C202" s="40">
         <v>1.05</v>
       </c>
-      <c r="D202" s="5">
+      <c r="D202" s="40">
         <v>1.46</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>167</v>
       </c>
-      <c r="B203" s="5">
+      <c r="B203" s="40">
         <v>1.44</v>
       </c>
-      <c r="C203" s="5">
+      <c r="C203" s="40">
         <v>1.31</v>
       </c>
-      <c r="D203" s="5">
+      <c r="D203" s="40">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B204" s="42">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B204" s="38">
         <v>29</v>
       </c>
-      <c r="C204" s="42">
+      <c r="C204" s="38">
         <v>27</v>
       </c>
-      <c r="D204" s="42">
+      <c r="D204" s="38">
         <v>28</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204" s="39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="8">
         <v>98</v>
       </c>
-      <c r="B205" s="5">
+      <c r="B205" s="40">
         <v>1.42</v>
       </c>
-      <c r="C205" s="5">
+      <c r="C205" s="40">
         <v>1.49</v>
       </c>
-      <c r="D205" s="5">
+      <c r="D205" s="40">
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="8">
         <v>100</v>
       </c>
-      <c r="B206" s="5">
+      <c r="B206" s="40">
         <v>2.1300000000000003</v>
       </c>
-      <c r="C206" s="5">
+      <c r="C206" s="40">
         <v>2.4700000000000002</v>
       </c>
-      <c r="D206" s="5">
+      <c r="D206" s="40">
         <v>0.96</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="6">
         <v>133</v>
       </c>
-      <c r="B207" s="5">
+      <c r="B207" s="40">
         <v>2.0900000000000003</v>
       </c>
-      <c r="C207" s="5">
+      <c r="C207" s="40">
         <v>2.31</v>
       </c>
-      <c r="D207" s="5">
+      <c r="D207" s="40">
         <v>0.73</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="6">
         <v>65</v>
       </c>
-      <c r="B208" s="5">
+      <c r="B208" s="40">
         <v>1.43</v>
       </c>
-      <c r="C208" s="5">
+      <c r="C208" s="40">
         <v>1.5899999999999999</v>
       </c>
-      <c r="D208" s="5">
+      <c r="D208" s="40">
         <v>1.1099999999999999</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="32">
+      <c r="A209" s="24">
         <v>1045</v>
       </c>
-      <c r="B209" s="5">
+      <c r="B209" s="40">
         <v>2.1500000000000004</v>
       </c>
-      <c r="C209" s="5">
+      <c r="C209" s="40">
         <v>2.31</v>
       </c>
-      <c r="D209" s="5">
+      <c r="D209" s="40">
         <v>0.59000000000000008</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="32">
+      <c r="A210" s="24">
         <v>1057</v>
       </c>
-      <c r="B210" s="5">
+      <c r="B210" s="40">
         <v>1.7499999999999998</v>
       </c>
-      <c r="C210" s="5">
+      <c r="C210" s="40">
         <v>1.8299999999999998</v>
       </c>
-      <c r="D210" s="5">
+      <c r="D210" s="40">
         <v>0.78</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="32">
+      <c r="A211" s="24">
         <v>1063</v>
       </c>
-      <c r="B211" s="5">
+      <c r="B211" s="40">
         <v>2.8000000000000003</v>
       </c>
-      <c r="C211" s="5">
+      <c r="C211" s="40">
         <v>3.08</v>
       </c>
-      <c r="D211" s="5">
+      <c r="D211" s="40">
         <v>1.84</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="32">
+      <c r="A212" s="24">
         <v>1041</v>
       </c>
-      <c r="B212" s="5">
+      <c r="B212" s="40">
         <v>1.84</v>
       </c>
-      <c r="C212" s="5">
+      <c r="C212" s="40">
         <v>1.8800000000000001</v>
       </c>
-      <c r="D212" s="5">
+      <c r="D212" s="40">
         <v>0.67999999999999994</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="37"/>
+      <c r="A213" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="H79:L79"/>
+    <mergeCell ref="M79:P79"/>
     <mergeCell ref="A183:D183"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A49:D49"/>
     <mergeCell ref="B79:D79"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="H79:L79"/>
-    <mergeCell ref="M79:P79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>